<commit_message>
Revert "Dichotic Finished (almost)"
This reverts commit a43f96dc2639f499a51175f1e7d20ed0e5d1c020.
</commit_message>
<xml_diff>
--- a/Data/Subject_1/Dichotic.xlsx
+++ b/Data/Subject_1/Dichotic.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="19">
   <si>
     <t>trial_side</t>
   </si>
@@ -49,16 +49,16 @@
     <t>block</t>
   </si>
   <si>
-    <t>sentence_id</t>
-  </si>
-  <si>
-    <t>Response</t>
+    <t>Left</t>
   </si>
   <si>
     <t>Right</t>
   </si>
   <si>
-    <t>Left</t>
+    <t>First Practice</t>
+  </si>
+  <si>
+    <t>Second Practice</t>
   </si>
   <si>
     <t>Real Trials</t>
@@ -428,13 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,37 +468,31 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
       <c r="F2">
-        <v>1582825701.899</v>
+        <v>1582822050.753</v>
       </c>
       <c r="G2">
-        <v>1582825704.604</v>
+        <v>1582822052.775</v>
       </c>
       <c r="H2">
-        <v>2393.333333333334</v>
+        <v>1708.004535147392</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -506,37 +500,31 @@
       <c r="L2">
         <v>0</v>
       </c>
-      <c r="M2">
-        <v>80</v>
-      </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3">
-        <v>1582825702.412</v>
+        <v>1582822052.775</v>
       </c>
       <c r="G3">
-        <v>1582825705.138</v>
+        <v>1582822055.324</v>
       </c>
       <c r="H3">
-        <v>2401.337868480726</v>
+        <v>2235.986394557823</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -544,37 +532,31 @@
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="M3">
-        <v>59</v>
-      </c>
-      <c r="N3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4">
-        <v>1582825704.604</v>
+        <v>1582822055.326</v>
       </c>
       <c r="G4">
-        <v>1582825706.628</v>
+        <v>1582822057.872</v>
       </c>
       <c r="H4">
-        <v>1715.986394557823</v>
+        <v>2228.004535147392</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -582,37 +564,31 @@
       <c r="L4">
         <v>0</v>
       </c>
-      <c r="M4">
-        <v>92</v>
-      </c>
-      <c r="N4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
-        <v>1582825705.138</v>
+        <v>1582822057.873</v>
       </c>
       <c r="G5">
-        <v>1582825707.67</v>
+        <v>1582822060.404</v>
       </c>
       <c r="H5">
-        <v>2222.65306122449</v>
+        <v>2228.004535147392</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
@@ -620,37 +596,31 @@
       <c r="L5">
         <v>0</v>
       </c>
-      <c r="M5">
-        <v>9</v>
-      </c>
-      <c r="N5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
       <c r="F6">
-        <v>1582825706.628</v>
+        <v>1582822060.406</v>
       </c>
       <c r="G6">
-        <v>1582825709.001</v>
+        <v>1582822062.613</v>
       </c>
       <c r="H6">
-        <v>2065.351473922902</v>
+        <v>1889.319727891156</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -658,37 +628,31 @@
       <c r="L6">
         <v>0</v>
       </c>
-      <c r="M6">
-        <v>91</v>
-      </c>
-      <c r="N6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>1582825707.67</v>
+        <v>1582822062.614</v>
       </c>
       <c r="G7">
-        <v>1582825710.226</v>
+        <v>1582822064.637</v>
       </c>
       <c r="H7">
-        <v>2233.333333333333</v>
+        <v>1713.333333333333</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
@@ -696,37 +660,31 @@
       <c r="L7">
         <v>0</v>
       </c>
-      <c r="M7">
-        <v>22</v>
-      </c>
-      <c r="N7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
       <c r="E8" t="s">
         <v>16</v>
       </c>
       <c r="F8">
-        <v>1582825709.001</v>
+        <v>1582822064.638</v>
       </c>
       <c r="G8">
-        <v>1582825711.21</v>
+        <v>1582822066.656</v>
       </c>
       <c r="H8">
-        <v>1889.319727891156</v>
+        <v>1713.333333333333</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
@@ -734,37 +692,31 @@
       <c r="L8">
         <v>0</v>
       </c>
-      <c r="M8">
-        <v>93</v>
-      </c>
-      <c r="N8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9">
-        <v>1582825710.226</v>
+        <v>1582822066.657</v>
       </c>
       <c r="G9">
-        <v>1582825712.601</v>
+        <v>1582822068.862</v>
       </c>
       <c r="H9">
-        <v>2052.018140589569</v>
+        <v>1886.666666666667</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -772,37 +724,31 @@
       <c r="L9">
         <v>0</v>
       </c>
-      <c r="M9">
-        <v>26</v>
-      </c>
-      <c r="N9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
       </c>
       <c r="F10">
-        <v>1582825711.21</v>
+        <v>1582822068.862</v>
       </c>
       <c r="G10">
-        <v>1582825713.564</v>
+        <v>1582822071.406</v>
       </c>
       <c r="H10">
-        <v>2049.319727891156</v>
+        <v>2228.004535147392</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
@@ -810,37 +756,31 @@
       <c r="L10">
         <v>0</v>
       </c>
-      <c r="M10">
-        <v>98</v>
-      </c>
-      <c r="N10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11">
-        <v>1582825712.601</v>
+        <v>1582822073.487</v>
       </c>
       <c r="G11">
-        <v>1582825714.972</v>
+        <v>1582822076.024</v>
       </c>
       <c r="H11">
-        <v>2052.018140589569</v>
+        <v>2230.680272108843</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
@@ -848,37 +788,31 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11">
-        <v>6</v>
-      </c>
-      <c r="N11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
       </c>
       <c r="F12">
-        <v>1582825713.564</v>
+        <v>1582822074.002</v>
       </c>
       <c r="G12">
-        <v>1582825715.935</v>
+        <v>1582822076.372</v>
       </c>
       <c r="H12">
-        <v>2049.319727891156</v>
+        <v>2062.65306122449</v>
       </c>
       <c r="I12" t="s">
         <v>18</v>
@@ -886,37 +820,31 @@
       <c r="L12">
         <v>0</v>
       </c>
-      <c r="M12">
-        <v>98</v>
-      </c>
-      <c r="N12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13">
-        <v>1582825714.972</v>
+        <v>1582822076.024</v>
       </c>
       <c r="G13">
-        <v>1582825717.673</v>
+        <v>1582822078.065</v>
       </c>
       <c r="H13">
-        <v>2393.333333333334</v>
+        <v>1726.666666666667</v>
       </c>
       <c r="I13" t="s">
         <v>18</v>
@@ -924,37 +852,31 @@
       <c r="L13">
         <v>0</v>
       </c>
-      <c r="M13">
-        <v>17</v>
-      </c>
-      <c r="N13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
       </c>
       <c r="F14">
-        <v>1582825715.935</v>
+        <v>1582822078.065</v>
       </c>
       <c r="G14">
-        <v>1582825717.963</v>
+        <v>1582822080.104</v>
       </c>
       <c r="H14">
-        <v>1713.333333333333</v>
+        <v>1726.666666666667</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
@@ -962,37 +884,31 @@
       <c r="L14">
         <v>0</v>
       </c>
-      <c r="M14">
-        <v>76</v>
-      </c>
-      <c r="N14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
       </c>
       <c r="F15">
-        <v>1582825717.963</v>
+        <v>1582822076.372</v>
       </c>
       <c r="G15">
-        <v>1582825720.005</v>
+        <v>1582822080.453</v>
       </c>
       <c r="H15">
-        <v>1726.666666666667</v>
+        <v>3772.018140589569</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1000,37 +916,31 @@
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15">
-        <v>81</v>
-      </c>
-      <c r="N15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16">
-        <v>1582825717.673</v>
+        <v>1582822080.104</v>
       </c>
       <c r="G16">
-        <v>1582825720.56</v>
+        <v>1582822082.31</v>
       </c>
       <c r="H16">
-        <v>2577.34693877551</v>
+        <v>1886.666666666667</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1038,37 +948,31 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16">
-        <v>10</v>
-      </c>
-      <c r="N16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
       </c>
       <c r="F17">
-        <v>1582825720.005</v>
+        <v>1582822080.453</v>
       </c>
       <c r="G17">
-        <v>1582825722.38</v>
+        <v>1582822084.532</v>
       </c>
       <c r="H17">
-        <v>2062.65306122449</v>
+        <v>3772.018140589569</v>
       </c>
       <c r="I17" t="s">
         <v>18</v>
@@ -1076,37 +980,31 @@
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17">
-        <v>86</v>
-      </c>
-      <c r="N17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18">
-        <v>1582825720.56</v>
+        <v>1582822084.532</v>
       </c>
       <c r="G18">
-        <v>1582825723.449</v>
+        <v>1582822087.064</v>
       </c>
       <c r="H18">
-        <v>2577.34693877551</v>
+        <v>2225.351473922903</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
@@ -1114,22 +1012,16 @@
       <c r="L18">
         <v>0</v>
       </c>
-      <c r="M18">
-        <v>10</v>
-      </c>
-      <c r="N18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -1138,13 +1030,13 @@
         <v>16</v>
       </c>
       <c r="F19">
-        <v>1582825722.38</v>
+        <v>1582822094.302</v>
       </c>
       <c r="G19">
-        <v>1582825724.76</v>
+        <v>1582822096.337</v>
       </c>
       <c r="H19">
-        <v>2062.65306122449</v>
+        <v>1726.666666666667</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
@@ -1152,22 +1044,16 @@
       <c r="L19">
         <v>0</v>
       </c>
-      <c r="M19">
-        <v>86</v>
-      </c>
-      <c r="N19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C20">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -1176,13 +1062,13 @@
         <v>17</v>
       </c>
       <c r="F20">
-        <v>1582825723.449</v>
+        <v>1582822094.803</v>
       </c>
       <c r="G20">
-        <v>1582825726.009</v>
+        <v>1582822098.36</v>
       </c>
       <c r="H20">
-        <v>2238.684807256236</v>
+        <v>3252.018140589569</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>
@@ -1190,22 +1076,16 @@
       <c r="L20">
         <v>0</v>
       </c>
-      <c r="M20">
-        <v>16</v>
-      </c>
-      <c r="N20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -1214,13 +1094,13 @@
         <v>16</v>
       </c>
       <c r="F21">
-        <v>1582825724.76</v>
+        <v>1582822096.337</v>
       </c>
       <c r="G21">
-        <v>1582825726.624</v>
+        <v>1582822098.365</v>
       </c>
       <c r="H21">
-        <v>1555.986394557823</v>
+        <v>1718.684807256236</v>
       </c>
       <c r="I21" t="s">
         <v>18</v>
@@ -1228,37 +1108,31 @@
       <c r="L21">
         <v>0</v>
       </c>
-      <c r="M21">
-        <v>70</v>
-      </c>
-      <c r="N21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22">
-        <v>1582825726.009</v>
+        <v>1582822098.365</v>
       </c>
       <c r="G22">
-        <v>1582825728.568</v>
+        <v>1582822100.914</v>
       </c>
       <c r="H22">
-        <v>2238.684807256236</v>
+        <v>2225.351473922903</v>
       </c>
       <c r="I22" t="s">
         <v>18</v>
@@ -1266,37 +1140,31 @@
       <c r="L22">
         <v>0</v>
       </c>
-      <c r="M22">
-        <v>16</v>
-      </c>
-      <c r="N22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
         <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F23">
-        <v>1582825726.624</v>
+        <v>1582822098.36</v>
       </c>
       <c r="G23">
-        <v>1582825729.164</v>
+        <v>1582822101.408</v>
       </c>
       <c r="H23">
-        <v>2230.680272108843</v>
+        <v>2742.65306122449</v>
       </c>
       <c r="I23" t="s">
         <v>18</v>
@@ -1304,37 +1172,31 @@
       <c r="L23">
         <v>0</v>
       </c>
-      <c r="M23">
-        <v>85</v>
-      </c>
-      <c r="N23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
         <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24">
-        <v>1582825728.568</v>
+        <v>1582822100.914</v>
       </c>
       <c r="G24">
-        <v>1582825731.288</v>
+        <v>1582822103.453</v>
       </c>
       <c r="H24">
-        <v>2406.666666666667</v>
+        <v>2225.351473922903</v>
       </c>
       <c r="I24" t="s">
         <v>18</v>
@@ -1342,22 +1204,16 @@
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="M24">
-        <v>48</v>
-      </c>
-      <c r="N24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -1366,13 +1222,13 @@
         <v>17</v>
       </c>
       <c r="F25">
-        <v>1582825731.288</v>
+        <v>1582822101.408</v>
       </c>
       <c r="G25">
-        <v>1582825734.17</v>
+        <v>1582822104.132</v>
       </c>
       <c r="H25">
-        <v>2566.666666666667</v>
+        <v>2401.337868480726</v>
       </c>
       <c r="I25" t="s">
         <v>18</v>
@@ -1380,10 +1236,548 @@
       <c r="L25">
         <v>0</v>
       </c>
-      <c r="M25">
-        <v>2</v>
-      </c>
-      <c r="N25" t="b">
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26">
+        <v>1582822103.453</v>
+      </c>
+      <c r="G26">
+        <v>1582822107.541</v>
+      </c>
+      <c r="H26">
+        <v>3772.018140589569</v>
+      </c>
+      <c r="I26" t="s">
+        <v>18</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27">
+        <v>1582822104.132</v>
+      </c>
+      <c r="G27">
+        <v>1582822107.709</v>
+      </c>
+      <c r="H27">
+        <v>3257.34693877551</v>
+      </c>
+      <c r="I27" t="s">
+        <v>18</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28">
+        <v>1582822107.541</v>
+      </c>
+      <c r="G28">
+        <v>1582822109.57</v>
+      </c>
+      <c r="H28">
+        <v>1708.004535147392</v>
+      </c>
+      <c r="I28" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <v>1582822107.709</v>
+      </c>
+      <c r="G29">
+        <v>1582822110.064</v>
+      </c>
+      <c r="H29">
+        <v>2052.018140589569</v>
+      </c>
+      <c r="I29" t="s">
+        <v>18</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <v>1582822109.57</v>
+      </c>
+      <c r="G30">
+        <v>1582822112.11</v>
+      </c>
+      <c r="H30">
+        <v>2235.986394557823</v>
+      </c>
+      <c r="I30" t="s">
+        <v>18</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>1582822110.064</v>
+      </c>
+      <c r="G31">
+        <v>1582822112.788</v>
+      </c>
+      <c r="H31">
+        <v>2406.666666666667</v>
+      </c>
+      <c r="I31" t="s">
+        <v>18</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>1582822112.11</v>
+      </c>
+      <c r="G32">
+        <v>1582822114.811</v>
+      </c>
+      <c r="H32">
+        <v>2393.333333333334</v>
+      </c>
+      <c r="I32" t="s">
+        <v>18</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33">
+        <v>1582822112.788</v>
+      </c>
+      <c r="G33">
+        <v>1582822115.508</v>
+      </c>
+      <c r="H33">
+        <v>2404.013605442177</v>
+      </c>
+      <c r="I33" t="s">
+        <v>18</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34">
+        <v>1582822114.811</v>
+      </c>
+      <c r="G34">
+        <v>1582822116.674</v>
+      </c>
+      <c r="H34">
+        <v>1555.986394557823</v>
+      </c>
+      <c r="I34" t="s">
+        <v>18</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35">
+        <v>1582822115.508</v>
+      </c>
+      <c r="G35">
+        <v>1582822118.23</v>
+      </c>
+      <c r="H35">
+        <v>2404.013605442177</v>
+      </c>
+      <c r="I35" t="s">
+        <v>18</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36">
+        <v>1582822116.674</v>
+      </c>
+      <c r="G36">
+        <v>1582822119.05</v>
+      </c>
+      <c r="H36">
+        <v>2065.351473922902</v>
+      </c>
+      <c r="I36" t="s">
+        <v>18</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37">
+        <v>1582822118.23</v>
+      </c>
+      <c r="G37">
+        <v>1582822120.606</v>
+      </c>
+      <c r="H37">
+        <v>2052.018140589569</v>
+      </c>
+      <c r="I37" t="s">
+        <v>18</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38">
+        <v>1582822119.05</v>
+      </c>
+      <c r="G38">
+        <v>1582822121.426</v>
+      </c>
+      <c r="H38">
+        <v>2065.351473922902</v>
+      </c>
+      <c r="I38" t="s">
+        <v>18</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39">
+        <v>1582822120.606</v>
+      </c>
+      <c r="G39">
+        <v>1582822122.98</v>
+      </c>
+      <c r="H39">
+        <v>2052.018140589569</v>
+      </c>
+      <c r="I39" t="s">
+        <v>18</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40">
+        <v>1582822121.426</v>
+      </c>
+      <c r="G40">
+        <v>1582822123.453</v>
+      </c>
+      <c r="H40">
+        <v>1713.333333333333</v>
+      </c>
+      <c r="I40" t="s">
+        <v>18</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41">
+        <v>1582822122.98</v>
+      </c>
+      <c r="G41">
+        <v>1582822125.513</v>
+      </c>
+      <c r="H41">
+        <v>2222.65306122449</v>
+      </c>
+      <c r="I41" t="s">
+        <v>18</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42">
+        <v>1582822125.513</v>
+      </c>
+      <c r="G42">
+        <v>1582822128.555</v>
+      </c>
+      <c r="H42">
+        <v>2734.671201814059</v>
+      </c>
+      <c r="I42" t="s">
+        <v>18</v>
+      </c>
+      <c r="L42">
         <v>0</v>
       </c>
     </row>

</xml_diff>